<commit_message>
chore: update prompt engineering Excel file to the latest version
</commit_message>
<xml_diff>
--- a/Documents/prompt engineering.xlsx
+++ b/Documents/prompt engineering.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\schema-mapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Downloads\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E765217-5A4D-4587-B659-930E29C31C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59962B03-8D04-4C74-A06E-0AF69973DC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -152,9 +152,6 @@
     <t>Follows schema and avoids extras.</t>
   </si>
   <si>
-    <t>Really good. to the point.</t>
-  </si>
-  <si>
     <t>remarks</t>
   </si>
   <si>
@@ -167,7 +164,10 @@
     <t>Type checks are creating a problem rest everything is workinging. Especially boolean</t>
   </si>
   <si>
-    <t>Perfect, but can reduce the usage to many tokens in the system prompt</t>
+    <t>Perfect</t>
+  </si>
+  <si>
+    <t>good but can do better</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -529,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -637,7 +637,7 @@
         <v>0.85</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -655,7 +655,7 @@
         <v>0.85</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -673,7 +673,7 @@
         <v>0.93</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="352.8" x14ac:dyDescent="0.3">
@@ -690,7 +690,7 @@
         <v>0.93</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -707,7 +707,7 @@
         <v>0.9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>